<commit_message>
Add test B and add train sample data with classify feature
</commit_message>
<xml_diff>
--- a/Data/test B/airport_city.xlsx
+++ b/Data/test B/airport_city.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sandra/TODO/机票航班延误预测算法大赛/Data/test B/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="467">
   <si>
     <t>AHJ</t>
   </si>
@@ -1418,13 +1429,20 @@
   </si>
   <si>
     <t>城市名称</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>林西</t>
+    <rPh sb="0" eb="1">
+      <t>lin'xi</t>
+    </rPh>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1766,11 +1784,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B235"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2975,6 +2993,9 @@
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>298</v>
+      </c>
+      <c r="B151" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>